<commit_message>
12042021 - Quasar All Atık
1- Cihaz veri akışı
2- Konteyner tanım detay
</commit_message>
<xml_diff>
--- a/Denemeler/Harita/All Atik/matrix-api/distance-matrix-response-converter/Distances.xlsx
+++ b/Denemeler/Harita/All Atik/matrix-api/distance-matrix-response-converter/Distances.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720ED0D6-88D5-4DD6-8C3C-C942DADF7CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4C6A1-9715-4DED-B72C-F13C6AB515C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19620" yWindow="270" windowWidth="8445" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distances" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -58,6 +58,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -110,6 +116,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -451,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,9 +474,10 @@
     <col min="1" max="1" width="11" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="14" max="22" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -498,7 +511,7 @@
       </c>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,8 +546,17 @@
         <v>1658</v>
       </c>
       <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="8">
+        <v>2</v>
+      </c>
+      <c r="O2" s="8">
+        <v>5</v>
+      </c>
+      <c r="P2" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -569,8 +591,17 @@
         <v>1166</v>
       </c>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="9">
+        <v>6</v>
+      </c>
+      <c r="O3" s="9">
+        <v>5</v>
+      </c>
+      <c r="P3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -606,7 +637,7 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -641,8 +672,20 @@
         <v>976</v>
       </c>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="8">
+        <v>2</v>
+      </c>
+      <c r="O5" s="8">
+        <v>5</v>
+      </c>
+      <c r="P5" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -677,8 +720,20 @@
         <v>1261</v>
       </c>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N6" s="9">
+        <v>6</v>
+      </c>
+      <c r="O6" s="9">
+        <v>8</v>
+      </c>
+      <c r="P6" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -714,7 +769,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -749,8 +804,32 @@
         <v>1262</v>
       </c>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
+        <v>2</v>
+      </c>
+      <c r="P8" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>4</v>
+      </c>
+      <c r="R8" s="8">
+        <v>5</v>
+      </c>
+      <c r="S8" s="8">
+        <v>6</v>
+      </c>
+      <c r="T8" s="8">
+        <v>7</v>
+      </c>
+      <c r="U8" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -785,8 +864,32 @@
         <v>987</v>
       </c>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="5">
+        <v>6</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>5</v>
+      </c>
+      <c r="R9" s="5">
+        <v>4</v>
+      </c>
+      <c r="S9" s="5">
+        <v>2</v>
+      </c>
+      <c r="T9" s="5">
+        <v>8</v>
+      </c>
+      <c r="U9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -822,7 +925,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
@@ -860,6 +963,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>